<commit_message>
Added Pin Usage Chart
</commit_message>
<xml_diff>
--- a/hardware/datasheets/Pins_Usage.xlsx
+++ b/hardware/datasheets/Pins_Usage.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Parker\Desktop\SeniorDesign\sddec21-07\hardware\datasheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{360FC926-D4E4-416C-8A16-6DDAE09D384B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E42C22-8F54-4DBF-9B4B-A04F87830E9F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5D8649F8-2B3A-427B-85BC-014C00AC5957}"/>
   </bookViews>
@@ -31,6 +31,206 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="65">
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Usage</t>
+  </si>
+  <si>
+    <t>Pin</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>BeagleBone P8</t>
+  </si>
+  <si>
+    <t>BeagleBone P9</t>
+  </si>
+  <si>
+    <t>GPIO_20</t>
+  </si>
+  <si>
+    <t>Lan_Heartbeat</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>All pins are currently tentative</t>
+  </si>
+  <si>
+    <t>Network_Connect</t>
+  </si>
+  <si>
+    <t>GPIO_48</t>
+  </si>
+  <si>
+    <t>SPI_CLK</t>
+  </si>
+  <si>
+    <t>SPI_MISO</t>
+  </si>
+  <si>
+    <t>SPI0_D0</t>
+  </si>
+  <si>
+    <t>SPI0_SCLK</t>
+  </si>
+  <si>
+    <t>SPI_MOSI</t>
+  </si>
+  <si>
+    <t>SPI0_D1</t>
+  </si>
+  <si>
+    <t>SPI0_CS0</t>
+  </si>
+  <si>
+    <t>SPI_CS</t>
+  </si>
+  <si>
+    <t>I2C2_SDA</t>
+  </si>
+  <si>
+    <t>I2C2_SCL</t>
+  </si>
+  <si>
+    <t>BeagleBone_Reset</t>
+  </si>
+  <si>
+    <t>SYS_RESETn</t>
+  </si>
+  <si>
+    <t>UART_TX</t>
+  </si>
+  <si>
+    <t>UART1_TXD</t>
+  </si>
+  <si>
+    <t>UART_RX</t>
+  </si>
+  <si>
+    <t>UART1_RXD</t>
+  </si>
+  <si>
+    <t>JTAG_..</t>
+  </si>
+  <si>
+    <t>2.4GHz P</t>
+  </si>
+  <si>
+    <t>2.4GHz N</t>
+  </si>
+  <si>
+    <t>2_4_GHZ_RF_P</t>
+  </si>
+  <si>
+    <t>2_4_GHZ_RF_N</t>
+  </si>
+  <si>
+    <t>Sub-1GHz P</t>
+  </si>
+  <si>
+    <t>Sub-1GHz N</t>
+  </si>
+  <si>
+    <t>SUB-1_GHZ_RF_P</t>
+  </si>
+  <si>
+    <t>SUB-1_GHZ_RF_N</t>
+  </si>
+  <si>
+    <t>DCDC_SW</t>
+  </si>
+  <si>
+    <t>RX_TX</t>
+  </si>
+  <si>
+    <t>CC1352 A</t>
+  </si>
+  <si>
+    <t>CC1352 B</t>
+  </si>
+  <si>
+    <t>DIO_3</t>
+  </si>
+  <si>
+    <t>DIO_4</t>
+  </si>
+  <si>
+    <t>DIO_5_HP</t>
+  </si>
+  <si>
+    <t>SPIO_MOSI</t>
+  </si>
+  <si>
+    <t>DIO_6_HP</t>
+  </si>
+  <si>
+    <t>DIO_7_HP</t>
+  </si>
+  <si>
+    <t>DIO_8</t>
+  </si>
+  <si>
+    <t>DIO_14</t>
+  </si>
+  <si>
+    <t>DIO_15</t>
+  </si>
+  <si>
+    <t>Zigbee_Connect</t>
+  </si>
+  <si>
+    <t>DIO_18</t>
+  </si>
+  <si>
+    <t>Check_Error</t>
+  </si>
+  <si>
+    <t>DIO_19</t>
+  </si>
+  <si>
+    <t>Zigbee_HeartBeat</t>
+  </si>
+  <si>
+    <t>DIO_20</t>
+  </si>
+  <si>
+    <t>Cape_HeartBeat</t>
+  </si>
+  <si>
+    <t>DIO_21</t>
+  </si>
+  <si>
+    <t>DIO_22</t>
+  </si>
+  <si>
+    <t>Aux_2</t>
+  </si>
+  <si>
+    <t>Aux_1</t>
+  </si>
+  <si>
+    <t>DIO_23_ANA</t>
+  </si>
+  <si>
+    <t>Button</t>
+  </si>
+  <si>
+    <t>LED</t>
+  </si>
+  <si>
+    <t>Programming</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -380,12 +580,491 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{048B8E6C-CB01-4B80-B999-98BA050B4B7A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="27.28515625" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" customWidth="1"/>
+    <col min="3" max="3" width="16.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.140625" customWidth="1"/>
+    <col min="5" max="5" width="73.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6">
+        <v>15</v>
+      </c>
+      <c r="E6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D10">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>20</v>
+      </c>
+      <c r="D11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16">
+        <v>35</v>
+      </c>
+      <c r="E16" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17">
+        <v>25</v>
+      </c>
+      <c r="E17" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B18" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" t="s">
+        <v>28</v>
+      </c>
+      <c r="D18">
+        <v>24</v>
+      </c>
+      <c r="E18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19">
+        <v>26</v>
+      </c>
+      <c r="E19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B20" t="s">
+        <v>28</v>
+      </c>
+      <c r="C20" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20">
+        <v>27</v>
+      </c>
+      <c r="E20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B22" t="s">
+        <v>30</v>
+      </c>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>33</v>
+      </c>
+      <c r="C23" t="s">
+        <v>35</v>
+      </c>
+      <c r="D23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B24" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" t="s">
+        <v>36</v>
+      </c>
+      <c r="D24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B25" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>37</v>
+      </c>
+      <c r="C26" t="s">
+        <v>37</v>
+      </c>
+      <c r="D26">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>40</v>
+      </c>
+      <c r="B28" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>43</v>
+      </c>
+      <c r="D30">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B31" t="s">
+        <v>44</v>
+      </c>
+      <c r="C31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B32" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B33" t="s">
+        <v>12</v>
+      </c>
+      <c r="C33" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>20</v>
+      </c>
+      <c r="C35" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>50</v>
+      </c>
+      <c r="C36" t="s">
+        <v>51</v>
+      </c>
+      <c r="D36">
+        <v>28</v>
+      </c>
+      <c r="E36" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C37" t="s">
+        <v>53</v>
+      </c>
+      <c r="D37">
+        <v>29</v>
+      </c>
+      <c r="E37" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B38" t="s">
+        <v>54</v>
+      </c>
+      <c r="C38" t="s">
+        <v>55</v>
+      </c>
+      <c r="D38">
+        <v>30</v>
+      </c>
+      <c r="E38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B39" t="s">
+        <v>56</v>
+      </c>
+      <c r="C39" t="s">
+        <v>57</v>
+      </c>
+      <c r="D39">
+        <v>31</v>
+      </c>
+      <c r="E39" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B40" t="s">
+        <v>59</v>
+      </c>
+      <c r="C40" t="s">
+        <v>58</v>
+      </c>
+      <c r="D40">
+        <v>32</v>
+      </c>
+      <c r="E40" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B41" t="s">
+        <v>60</v>
+      </c>
+      <c r="C41" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41">
+        <v>36</v>
+      </c>
+      <c r="E41" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>